<commit_message>
fixed column name bug
</commit_message>
<xml_diff>
--- a/app/data/chariot_race.xlsx
+++ b/app/data/chariot_race.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tudor\Desktop\grepolympia-calculator\app\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B1AA8D-15D7-4028-B044-5DB3F603D1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,14 +34,14 @@
     <t>Control</t>
   </si>
   <si>
-    <t>Score +/-5%</t>
+    <t>Score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +104,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,7 +156,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -176,6 +190,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -210,9 +225,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -385,14 +401,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,7 +427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -426,7 +444,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -443,7 +461,7 @@
         <v>2290</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -460,7 +478,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -474,10 +492,10 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>2444.97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>2444.9699999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -491,10 +509,10 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>2501.18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>2501.1799999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -511,7 +529,7 @@
         <v>2552.39</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -528,7 +546,7 @@
         <v>2602.39</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -545,7 +563,7 @@
         <v>2650.37</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -562,7 +580,7 @@
         <v>2694.29</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -579,7 +597,7 @@
         <v>2737.61</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -596,7 +614,7 @@
         <v>2777.76</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -613,7 +631,7 @@
         <v>2817.89</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -630,7 +648,7 @@
         <v>2857.07</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -647,7 +665,7 @@
         <v>2894.87</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -664,7 +682,7 @@
         <v>2931.96</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -681,7 +699,7 @@
         <v>2967.9</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -698,7 +716,7 @@
         <v>3003.69</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -715,7 +733,7 @@
         <v>3038.93</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -732,7 +750,7 @@
         <v>3073.36</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -749,7 +767,7 @@
         <v>3107.29</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -766,7 +784,7 @@
         <v>3140.47</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -783,7 +801,7 @@
         <v>3173.63</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -800,7 +818,7 @@
         <v>3206.55</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -817,7 +835,7 @@
         <v>3238.65</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -834,7 +852,7 @@
         <v>3270.72</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -851,7 +869,7 @@
         <v>3302.14</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -868,7 +886,7 @@
         <v>3333.26</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -885,7 +903,7 @@
         <v>3364.37</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -902,7 +920,7 @@
         <v>3395.21</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -919,7 +937,7 @@
         <v>3425.53</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -936,7 +954,7 @@
         <v>3455.81</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -953,7 +971,7 @@
         <v>3485.68</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -970,7 +988,7 @@
         <v>3515.21</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -987,7 +1005,7 @@
         <v>3544.68</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1004,7 +1022,7 @@
         <v>3574.08</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1021,7 +1039,7 @@
         <v>3603.18</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1038,7 +1056,7 @@
         <v>3632.04</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1055,7 +1073,7 @@
         <v>3660.81</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1072,7 +1090,7 @@
         <v>3689.26</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1089,7 +1107,7 @@
         <v>3717.51</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1106,7 +1124,7 @@
         <v>3745.68</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1123,7 +1141,7 @@
         <v>3773.65</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1140,7 +1158,7 @@
         <v>3801.56</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1157,7 +1175,7 @@
         <v>3829.25</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1174,7 +1192,7 @@
         <v>3856.92</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1191,7 +1209,7 @@
         <v>3884.35</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1208,7 +1226,7 @@
         <v>3911.57</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1225,7 +1243,7 @@
         <v>3938.74</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1242,7 +1260,7 @@
         <v>3965.76</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1259,7 +1277,7 @@
         <v>3992.58</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
fixed column name bugs
</commit_message>
<xml_diff>
--- a/app/data/chariot_race.xlsx
+++ b/app/data/chariot_race.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tudor\Desktop\grepolympia-calculator\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B1AA8D-15D7-4028-B044-5DB3F603D1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F733614-9491-4E5B-8E9C-E42BD92262B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -404,11 +404,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
added better excel with data
</commit_message>
<xml_diff>
--- a/app/data/chariot_race.xlsx
+++ b/app/data/chariot_race.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tudor\Desktop\grepolympia-calculator\app\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F733614-9491-4E5B-8E9C-E42BD92262B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -34,14 +28,14 @@
     <t>Control</t>
   </si>
   <si>
-    <t>Score</t>
+    <t>Score +/-5%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,21 +98,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -156,7 +142,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -190,7 +176,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -225,10 +210,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -401,18 +385,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>0</v>
       </c>
@@ -446,7 +426,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -463,7 +443,7 @@
         <v>2290</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>2</v>
       </c>
@@ -480,7 +460,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -494,10 +474,10 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>2444.9699999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2444.97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>4</v>
       </c>
@@ -511,10 +491,10 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>2501.1799999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2501.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>5</v>
       </c>
@@ -531,7 +511,7 @@
         <v>2552.39</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>6</v>
       </c>
@@ -548,7 +528,7 @@
         <v>2602.39</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>7</v>
       </c>
@@ -565,7 +545,7 @@
         <v>2650.37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>8</v>
       </c>
@@ -582,7 +562,7 @@
         <v>2694.29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>9</v>
       </c>
@@ -599,7 +579,7 @@
         <v>2737.61</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>10</v>
       </c>
@@ -616,7 +596,7 @@
         <v>2777.76</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>11</v>
       </c>
@@ -633,7 +613,7 @@
         <v>2817.89</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>12</v>
       </c>
@@ -650,7 +630,7 @@
         <v>2857.07</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>13</v>
       </c>
@@ -667,7 +647,7 @@
         <v>2894.87</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>14</v>
       </c>
@@ -684,7 +664,7 @@
         <v>2931.96</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>15</v>
       </c>
@@ -701,7 +681,7 @@
         <v>2967.9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>16</v>
       </c>
@@ -718,7 +698,7 @@
         <v>3003.69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>17</v>
       </c>
@@ -735,7 +715,7 @@
         <v>3038.93</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>18</v>
       </c>
@@ -752,7 +732,7 @@
         <v>3073.36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>19</v>
       </c>
@@ -769,7 +749,7 @@
         <v>3107.29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>20</v>
       </c>
@@ -786,7 +766,7 @@
         <v>3140.47</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>21</v>
       </c>
@@ -803,7 +783,7 @@
         <v>3173.63</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>22</v>
       </c>
@@ -820,7 +800,7 @@
         <v>3206.55</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>23</v>
       </c>
@@ -837,7 +817,7 @@
         <v>3238.65</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>24</v>
       </c>
@@ -854,7 +834,7 @@
         <v>3270.72</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>25</v>
       </c>
@@ -871,7 +851,7 @@
         <v>3302.14</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>26</v>
       </c>
@@ -888,7 +868,7 @@
         <v>3333.26</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>27</v>
       </c>
@@ -905,7 +885,7 @@
         <v>3364.37</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>28</v>
       </c>
@@ -922,7 +902,7 @@
         <v>3395.21</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>29</v>
       </c>
@@ -939,7 +919,7 @@
         <v>3425.53</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>30</v>
       </c>
@@ -956,7 +936,7 @@
         <v>3455.81</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>31</v>
       </c>
@@ -973,7 +953,7 @@
         <v>3485.68</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>32</v>
       </c>
@@ -990,7 +970,7 @@
         <v>3515.21</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1007,7 +987,7 @@
         <v>3544.68</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1024,7 +1004,7 @@
         <v>3574.08</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1041,7 +1021,7 @@
         <v>3603.18</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1058,7 +1038,7 @@
         <v>3632.04</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1075,7 +1055,7 @@
         <v>3660.81</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1092,7 +1072,7 @@
         <v>3689.26</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1109,7 +1089,7 @@
         <v>3717.51</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1126,7 +1106,7 @@
         <v>3745.68</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1143,7 +1123,7 @@
         <v>3773.65</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1160,7 +1140,7 @@
         <v>3801.56</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1177,7 +1157,7 @@
         <v>3829.25</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1194,7 +1174,7 @@
         <v>3856.92</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1211,7 +1191,7 @@
         <v>3884.35</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1228,7 +1208,7 @@
         <v>3911.57</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1245,7 +1225,7 @@
         <v>3938.74</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1262,7 +1242,7 @@
         <v>3965.76</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1279,7 +1259,7 @@
         <v>3992.58</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1294,6 +1274,3389 @@
       </c>
       <c r="E52">
         <v>4019.32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <v>22</v>
+      </c>
+      <c r="D53">
+        <v>18</v>
+      </c>
+      <c r="E53">
+        <v>4046.02</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>11</v>
+      </c>
+      <c r="C54">
+        <v>23</v>
+      </c>
+      <c r="D54">
+        <v>18</v>
+      </c>
+      <c r="E54">
+        <v>4072.66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>11</v>
+      </c>
+      <c r="C55">
+        <v>24</v>
+      </c>
+      <c r="D55">
+        <v>18</v>
+      </c>
+      <c r="E55">
+        <v>4099.13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>11</v>
+      </c>
+      <c r="C56">
+        <v>25</v>
+      </c>
+      <c r="D56">
+        <v>18</v>
+      </c>
+      <c r="E56">
+        <v>4125.43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <v>25</v>
+      </c>
+      <c r="D57">
+        <v>19</v>
+      </c>
+      <c r="E57">
+        <v>4151.68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>11</v>
+      </c>
+      <c r="C58">
+        <v>26</v>
+      </c>
+      <c r="D58">
+        <v>19</v>
+      </c>
+      <c r="E58">
+        <v>4177.83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>11</v>
+      </c>
+      <c r="C59">
+        <v>27</v>
+      </c>
+      <c r="D59">
+        <v>19</v>
+      </c>
+      <c r="E59">
+        <v>4203.83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>11</v>
+      </c>
+      <c r="C60">
+        <v>28</v>
+      </c>
+      <c r="D60">
+        <v>19</v>
+      </c>
+      <c r="E60">
+        <v>4229.68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>11</v>
+      </c>
+      <c r="C61">
+        <v>28</v>
+      </c>
+      <c r="D61">
+        <v>20</v>
+      </c>
+      <c r="E61">
+        <v>4255.52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>11</v>
+      </c>
+      <c r="C62">
+        <v>29</v>
+      </c>
+      <c r="D62">
+        <v>20</v>
+      </c>
+      <c r="E62">
+        <v>4281.24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>12</v>
+      </c>
+      <c r="C63">
+        <v>29</v>
+      </c>
+      <c r="D63">
+        <v>20</v>
+      </c>
+      <c r="E63">
+        <v>4306.9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>12</v>
+      </c>
+      <c r="C64">
+        <v>30</v>
+      </c>
+      <c r="D64">
+        <v>20</v>
+      </c>
+      <c r="E64">
+        <v>4332.48</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>12</v>
+      </c>
+      <c r="C65">
+        <v>30</v>
+      </c>
+      <c r="D65">
+        <v>21</v>
+      </c>
+      <c r="E65">
+        <v>4357.94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>12</v>
+      </c>
+      <c r="C66">
+        <v>31</v>
+      </c>
+      <c r="D66">
+        <v>21</v>
+      </c>
+      <c r="E66">
+        <v>4383.39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>12</v>
+      </c>
+      <c r="C67">
+        <v>32</v>
+      </c>
+      <c r="D67">
+        <v>21</v>
+      </c>
+      <c r="E67">
+        <v>4408.72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>12</v>
+      </c>
+      <c r="C68">
+        <v>33</v>
+      </c>
+      <c r="D68">
+        <v>21</v>
+      </c>
+      <c r="E68">
+        <v>4433.93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>12</v>
+      </c>
+      <c r="C69">
+        <v>34</v>
+      </c>
+      <c r="D69">
+        <v>21</v>
+      </c>
+      <c r="E69">
+        <v>4459.03</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>12</v>
+      </c>
+      <c r="C70">
+        <v>34</v>
+      </c>
+      <c r="D70">
+        <v>22</v>
+      </c>
+      <c r="E70">
+        <v>4484.13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>12</v>
+      </c>
+      <c r="C71">
+        <v>35</v>
+      </c>
+      <c r="D71">
+        <v>22</v>
+      </c>
+      <c r="E71">
+        <v>4509.11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>12</v>
+      </c>
+      <c r="C72">
+        <v>36</v>
+      </c>
+      <c r="D72">
+        <v>22</v>
+      </c>
+      <c r="E72">
+        <v>4533.99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>12</v>
+      </c>
+      <c r="C73">
+        <v>37</v>
+      </c>
+      <c r="D73">
+        <v>22</v>
+      </c>
+      <c r="E73">
+        <v>4558.77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>12</v>
+      </c>
+      <c r="C74">
+        <v>37</v>
+      </c>
+      <c r="D74">
+        <v>23</v>
+      </c>
+      <c r="E74">
+        <v>4583.53</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>13</v>
+      </c>
+      <c r="C75">
+        <v>37</v>
+      </c>
+      <c r="D75">
+        <v>23</v>
+      </c>
+      <c r="E75">
+        <v>4608.24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>13</v>
+      </c>
+      <c r="C76">
+        <v>38</v>
+      </c>
+      <c r="D76">
+        <v>23</v>
+      </c>
+      <c r="E76">
+        <v>4632.92</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>13</v>
+      </c>
+      <c r="C77">
+        <v>39</v>
+      </c>
+      <c r="D77">
+        <v>23</v>
+      </c>
+      <c r="E77">
+        <v>4657.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>13</v>
+      </c>
+      <c r="C78">
+        <v>40</v>
+      </c>
+      <c r="D78">
+        <v>23</v>
+      </c>
+      <c r="E78">
+        <v>4681.98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>13</v>
+      </c>
+      <c r="C79">
+        <v>40</v>
+      </c>
+      <c r="D79">
+        <v>24</v>
+      </c>
+      <c r="E79">
+        <v>4706.42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>13</v>
+      </c>
+      <c r="C80">
+        <v>41</v>
+      </c>
+      <c r="D80">
+        <v>24</v>
+      </c>
+      <c r="E80">
+        <v>4730.81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>13</v>
+      </c>
+      <c r="C81">
+        <v>42</v>
+      </c>
+      <c r="D81">
+        <v>24</v>
+      </c>
+      <c r="E81">
+        <v>4755.12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>13</v>
+      </c>
+      <c r="C82">
+        <v>43</v>
+      </c>
+      <c r="D82">
+        <v>24</v>
+      </c>
+      <c r="E82">
+        <v>4779.34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>13</v>
+      </c>
+      <c r="C83">
+        <v>44</v>
+      </c>
+      <c r="D83">
+        <v>24</v>
+      </c>
+      <c r="E83">
+        <v>4803.47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>13</v>
+      </c>
+      <c r="C84">
+        <v>44</v>
+      </c>
+      <c r="D84">
+        <v>25</v>
+      </c>
+      <c r="E84">
+        <v>4827.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>13</v>
+      </c>
+      <c r="C85">
+        <v>45</v>
+      </c>
+      <c r="D85">
+        <v>25</v>
+      </c>
+      <c r="E85">
+        <v>4851.65</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>13</v>
+      </c>
+      <c r="C86">
+        <v>46</v>
+      </c>
+      <c r="D86">
+        <v>25</v>
+      </c>
+      <c r="E86">
+        <v>4875.62</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>13</v>
+      </c>
+      <c r="C87">
+        <v>47</v>
+      </c>
+      <c r="D87">
+        <v>25</v>
+      </c>
+      <c r="E87">
+        <v>4899.52</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>14</v>
+      </c>
+      <c r="C88">
+        <v>47</v>
+      </c>
+      <c r="D88">
+        <v>25</v>
+      </c>
+      <c r="E88">
+        <v>4923.39</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>14</v>
+      </c>
+      <c r="C89">
+        <v>47</v>
+      </c>
+      <c r="D89">
+        <v>26</v>
+      </c>
+      <c r="E89">
+        <v>4947.24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>14</v>
+      </c>
+      <c r="C90">
+        <v>48</v>
+      </c>
+      <c r="D90">
+        <v>26</v>
+      </c>
+      <c r="E90">
+        <v>4971.05</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>14</v>
+      </c>
+      <c r="C91">
+        <v>49</v>
+      </c>
+      <c r="D91">
+        <v>26</v>
+      </c>
+      <c r="E91">
+        <v>4994.79</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>14</v>
+      </c>
+      <c r="C92">
+        <v>50</v>
+      </c>
+      <c r="D92">
+        <v>26</v>
+      </c>
+      <c r="E92">
+        <v>5018.46</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>14</v>
+      </c>
+      <c r="C93">
+        <v>51</v>
+      </c>
+      <c r="D93">
+        <v>26</v>
+      </c>
+      <c r="E93">
+        <v>5042.06</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>14</v>
+      </c>
+      <c r="C94">
+        <v>51</v>
+      </c>
+      <c r="D94">
+        <v>27</v>
+      </c>
+      <c r="E94">
+        <v>5065.63</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>14</v>
+      </c>
+      <c r="C95">
+        <v>52</v>
+      </c>
+      <c r="D95">
+        <v>27</v>
+      </c>
+      <c r="E95">
+        <v>5089.16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>14</v>
+      </c>
+      <c r="C96">
+        <v>53</v>
+      </c>
+      <c r="D96">
+        <v>27</v>
+      </c>
+      <c r="E96">
+        <v>5112.63</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>14</v>
+      </c>
+      <c r="C97">
+        <v>54</v>
+      </c>
+      <c r="D97">
+        <v>27</v>
+      </c>
+      <c r="E97">
+        <v>5136.02</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>14</v>
+      </c>
+      <c r="C98">
+        <v>55</v>
+      </c>
+      <c r="D98">
+        <v>27</v>
+      </c>
+      <c r="E98">
+        <v>5159.35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>14</v>
+      </c>
+      <c r="C99">
+        <v>55</v>
+      </c>
+      <c r="D99">
+        <v>28</v>
+      </c>
+      <c r="E99">
+        <v>5182.66</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>14</v>
+      </c>
+      <c r="C100">
+        <v>56</v>
+      </c>
+      <c r="D100">
+        <v>28</v>
+      </c>
+      <c r="E100">
+        <v>5205.93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>14</v>
+      </c>
+      <c r="C101">
+        <v>57</v>
+      </c>
+      <c r="D101">
+        <v>28</v>
+      </c>
+      <c r="E101">
+        <v>5229.14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>14</v>
+      </c>
+      <c r="C102">
+        <v>58</v>
+      </c>
+      <c r="D102">
+        <v>28</v>
+      </c>
+      <c r="E102">
+        <v>5252.28</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <v>15</v>
+      </c>
+      <c r="C103">
+        <v>58</v>
+      </c>
+      <c r="D103">
+        <v>28</v>
+      </c>
+      <c r="E103">
+        <v>5275.4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104">
+        <v>15</v>
+      </c>
+      <c r="C104">
+        <v>59</v>
+      </c>
+      <c r="D104">
+        <v>28</v>
+      </c>
+      <c r="E104">
+        <v>5298.48</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>15</v>
+      </c>
+      <c r="C105">
+        <v>59</v>
+      </c>
+      <c r="D105">
+        <v>29</v>
+      </c>
+      <c r="E105">
+        <v>5321.54</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106">
+        <v>15</v>
+      </c>
+      <c r="C106">
+        <v>60</v>
+      </c>
+      <c r="D106">
+        <v>29</v>
+      </c>
+      <c r="E106">
+        <v>5344.57</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107">
+        <v>15</v>
+      </c>
+      <c r="C107">
+        <v>61</v>
+      </c>
+      <c r="D107">
+        <v>29</v>
+      </c>
+      <c r="E107">
+        <v>5367.54</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108">
+        <v>15</v>
+      </c>
+      <c r="C108">
+        <v>62</v>
+      </c>
+      <c r="D108">
+        <v>29</v>
+      </c>
+      <c r="E108">
+        <v>5390.45</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109">
+        <v>15</v>
+      </c>
+      <c r="C109">
+        <v>63</v>
+      </c>
+      <c r="D109">
+        <v>29</v>
+      </c>
+      <c r="E109">
+        <v>5413.31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110">
+        <v>15</v>
+      </c>
+      <c r="C110">
+        <v>63</v>
+      </c>
+      <c r="D110">
+        <v>30</v>
+      </c>
+      <c r="E110">
+        <v>5436.13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111">
+        <v>15</v>
+      </c>
+      <c r="C111">
+        <v>64</v>
+      </c>
+      <c r="D111">
+        <v>30</v>
+      </c>
+      <c r="E111">
+        <v>5458.93</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112">
+        <v>15</v>
+      </c>
+      <c r="C112">
+        <v>65</v>
+      </c>
+      <c r="D112">
+        <v>30</v>
+      </c>
+      <c r="E112">
+        <v>5481.68</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113">
+        <v>15</v>
+      </c>
+      <c r="C113">
+        <v>66</v>
+      </c>
+      <c r="D113">
+        <v>30</v>
+      </c>
+      <c r="E113">
+        <v>5504.38</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114">
+        <v>15</v>
+      </c>
+      <c r="C114">
+        <v>67</v>
+      </c>
+      <c r="D114">
+        <v>30</v>
+      </c>
+      <c r="E114">
+        <v>5527.02</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115">
+        <v>15</v>
+      </c>
+      <c r="C115">
+        <v>67</v>
+      </c>
+      <c r="D115">
+        <v>31</v>
+      </c>
+      <c r="E115">
+        <v>5549.62</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116">
+        <v>15</v>
+      </c>
+      <c r="C116">
+        <v>68</v>
+      </c>
+      <c r="D116">
+        <v>31</v>
+      </c>
+      <c r="E116">
+        <v>5572.21</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117">
+        <v>15</v>
+      </c>
+      <c r="C117">
+        <v>69</v>
+      </c>
+      <c r="D117">
+        <v>31</v>
+      </c>
+      <c r="E117">
+        <v>5594.76</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118">
+        <v>15</v>
+      </c>
+      <c r="C118">
+        <v>70</v>
+      </c>
+      <c r="D118">
+        <v>31</v>
+      </c>
+      <c r="E118">
+        <v>5617.25</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119">
+        <v>117</v>
+      </c>
+      <c r="B119">
+        <v>15</v>
+      </c>
+      <c r="C119">
+        <v>71</v>
+      </c>
+      <c r="D119">
+        <v>31</v>
+      </c>
+      <c r="E119">
+        <v>5639.7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120">
+        <v>16</v>
+      </c>
+      <c r="C120">
+        <v>71</v>
+      </c>
+      <c r="D120">
+        <v>31</v>
+      </c>
+      <c r="E120">
+        <v>5662.13</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121">
+        <v>16</v>
+      </c>
+      <c r="C121">
+        <v>72</v>
+      </c>
+      <c r="D121">
+        <v>31</v>
+      </c>
+      <c r="E121">
+        <v>5684.53</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122">
+        <v>16</v>
+      </c>
+      <c r="C122">
+        <v>72</v>
+      </c>
+      <c r="D122">
+        <v>32</v>
+      </c>
+      <c r="E122">
+        <v>5706.91</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123">
+        <v>16</v>
+      </c>
+      <c r="C123">
+        <v>73</v>
+      </c>
+      <c r="D123">
+        <v>32</v>
+      </c>
+      <c r="E123">
+        <v>5729.27</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="B124">
+        <v>16</v>
+      </c>
+      <c r="C124">
+        <v>74</v>
+      </c>
+      <c r="D124">
+        <v>32</v>
+      </c>
+      <c r="E124">
+        <v>5751.57</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125">
+        <v>16</v>
+      </c>
+      <c r="C125">
+        <v>75</v>
+      </c>
+      <c r="D125">
+        <v>32</v>
+      </c>
+      <c r="E125">
+        <v>5773.84</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126">
+        <v>16</v>
+      </c>
+      <c r="C126">
+        <v>76</v>
+      </c>
+      <c r="D126">
+        <v>32</v>
+      </c>
+      <c r="E126">
+        <v>5796.05</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127">
+        <v>16</v>
+      </c>
+      <c r="C127">
+        <v>77</v>
+      </c>
+      <c r="D127">
+        <v>32</v>
+      </c>
+      <c r="E127">
+        <v>5818.23</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128">
+        <v>16</v>
+      </c>
+      <c r="C128">
+        <v>77</v>
+      </c>
+      <c r="D128">
+        <v>33</v>
+      </c>
+      <c r="E128">
+        <v>5840.4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129">
+        <v>16</v>
+      </c>
+      <c r="C129">
+        <v>78</v>
+      </c>
+      <c r="D129">
+        <v>33</v>
+      </c>
+      <c r="E129">
+        <v>5862.53</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130">
+        <v>128</v>
+      </c>
+      <c r="B130">
+        <v>16</v>
+      </c>
+      <c r="C130">
+        <v>79</v>
+      </c>
+      <c r="D130">
+        <v>33</v>
+      </c>
+      <c r="E130">
+        <v>5884.62</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131">
+        <v>129</v>
+      </c>
+      <c r="B131">
+        <v>16</v>
+      </c>
+      <c r="C131">
+        <v>80</v>
+      </c>
+      <c r="D131">
+        <v>33</v>
+      </c>
+      <c r="E131">
+        <v>5906.66</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132">
+        <v>130</v>
+      </c>
+      <c r="B132">
+        <v>16</v>
+      </c>
+      <c r="C132">
+        <v>81</v>
+      </c>
+      <c r="D132">
+        <v>33</v>
+      </c>
+      <c r="E132">
+        <v>5928.67</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133">
+        <v>131</v>
+      </c>
+      <c r="B133">
+        <v>16</v>
+      </c>
+      <c r="C133">
+        <v>81</v>
+      </c>
+      <c r="D133">
+        <v>34</v>
+      </c>
+      <c r="E133">
+        <v>5950.64</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134">
+        <v>132</v>
+      </c>
+      <c r="B134">
+        <v>16</v>
+      </c>
+      <c r="C134">
+        <v>82</v>
+      </c>
+      <c r="D134">
+        <v>34</v>
+      </c>
+      <c r="E134">
+        <v>5972.6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135">
+        <v>133</v>
+      </c>
+      <c r="B135">
+        <v>16</v>
+      </c>
+      <c r="C135">
+        <v>83</v>
+      </c>
+      <c r="D135">
+        <v>34</v>
+      </c>
+      <c r="E135">
+        <v>5994.53</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136">
+        <v>134</v>
+      </c>
+      <c r="B136">
+        <v>16</v>
+      </c>
+      <c r="C136">
+        <v>84</v>
+      </c>
+      <c r="D136">
+        <v>34</v>
+      </c>
+      <c r="E136">
+        <v>6016.41</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137">
+        <v>135</v>
+      </c>
+      <c r="B137">
+        <v>16</v>
+      </c>
+      <c r="C137">
+        <v>85</v>
+      </c>
+      <c r="D137">
+        <v>34</v>
+      </c>
+      <c r="E137">
+        <v>6038.26</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138">
+        <v>136</v>
+      </c>
+      <c r="B138">
+        <v>17</v>
+      </c>
+      <c r="C138">
+        <v>85</v>
+      </c>
+      <c r="D138">
+        <v>34</v>
+      </c>
+      <c r="E138">
+        <v>6060.07</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139">
+        <v>137</v>
+      </c>
+      <c r="B139">
+        <v>17</v>
+      </c>
+      <c r="C139">
+        <v>86</v>
+      </c>
+      <c r="D139">
+        <v>34</v>
+      </c>
+      <c r="E139">
+        <v>6081.87</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140">
+        <v>138</v>
+      </c>
+      <c r="B140">
+        <v>17</v>
+      </c>
+      <c r="C140">
+        <v>86</v>
+      </c>
+      <c r="D140">
+        <v>35</v>
+      </c>
+      <c r="E140">
+        <v>6103.65</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141">
+        <v>139</v>
+      </c>
+      <c r="B141">
+        <v>17</v>
+      </c>
+      <c r="C141">
+        <v>87</v>
+      </c>
+      <c r="D141">
+        <v>35</v>
+      </c>
+      <c r="E141">
+        <v>6125.42</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142">
+        <v>140</v>
+      </c>
+      <c r="B142">
+        <v>17</v>
+      </c>
+      <c r="C142">
+        <v>88</v>
+      </c>
+      <c r="D142">
+        <v>35</v>
+      </c>
+      <c r="E142">
+        <v>6147.15</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143">
+        <v>141</v>
+      </c>
+      <c r="B143">
+        <v>17</v>
+      </c>
+      <c r="C143">
+        <v>89</v>
+      </c>
+      <c r="D143">
+        <v>35</v>
+      </c>
+      <c r="E143">
+        <v>6168.84</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144">
+        <v>142</v>
+      </c>
+      <c r="B144">
+        <v>17</v>
+      </c>
+      <c r="C144">
+        <v>90</v>
+      </c>
+      <c r="D144">
+        <v>35</v>
+      </c>
+      <c r="E144">
+        <v>6190.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>17</v>
+      </c>
+      <c r="C145">
+        <v>91</v>
+      </c>
+      <c r="D145">
+        <v>35</v>
+      </c>
+      <c r="E145">
+        <v>6212.12</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146">
+        <v>144</v>
+      </c>
+      <c r="B146">
+        <v>17</v>
+      </c>
+      <c r="C146">
+        <v>91</v>
+      </c>
+      <c r="D146">
+        <v>36</v>
+      </c>
+      <c r="E146">
+        <v>6233.72</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147">
+        <v>145</v>
+      </c>
+      <c r="B147">
+        <v>17</v>
+      </c>
+      <c r="C147">
+        <v>92</v>
+      </c>
+      <c r="D147">
+        <v>36</v>
+      </c>
+      <c r="E147">
+        <v>6255.3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148">
+        <v>146</v>
+      </c>
+      <c r="B148">
+        <v>17</v>
+      </c>
+      <c r="C148">
+        <v>93</v>
+      </c>
+      <c r="D148">
+        <v>36</v>
+      </c>
+      <c r="E148">
+        <v>6276.85</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149">
+        <v>147</v>
+      </c>
+      <c r="B149">
+        <v>17</v>
+      </c>
+      <c r="C149">
+        <v>94</v>
+      </c>
+      <c r="D149">
+        <v>36</v>
+      </c>
+      <c r="E149">
+        <v>6298.37</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150">
+        <v>148</v>
+      </c>
+      <c r="B150">
+        <v>17</v>
+      </c>
+      <c r="C150">
+        <v>95</v>
+      </c>
+      <c r="D150">
+        <v>36</v>
+      </c>
+      <c r="E150">
+        <v>6319.85</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151">
+        <v>149</v>
+      </c>
+      <c r="B151">
+        <v>17</v>
+      </c>
+      <c r="C151">
+        <v>96</v>
+      </c>
+      <c r="D151">
+        <v>36</v>
+      </c>
+      <c r="E151">
+        <v>6341.3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152">
+        <v>150</v>
+      </c>
+      <c r="B152">
+        <v>17</v>
+      </c>
+      <c r="C152">
+        <v>97</v>
+      </c>
+      <c r="D152">
+        <v>36</v>
+      </c>
+      <c r="E152">
+        <v>6362.71</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153">
+        <v>151</v>
+      </c>
+      <c r="B153">
+        <v>17</v>
+      </c>
+      <c r="C153">
+        <v>97</v>
+      </c>
+      <c r="D153">
+        <v>37</v>
+      </c>
+      <c r="E153">
+        <v>6384.13</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154">
+        <v>152</v>
+      </c>
+      <c r="B154">
+        <v>17</v>
+      </c>
+      <c r="C154">
+        <v>98</v>
+      </c>
+      <c r="D154">
+        <v>37</v>
+      </c>
+      <c r="E154">
+        <v>6405.51</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155">
+        <v>153</v>
+      </c>
+      <c r="B155">
+        <v>17</v>
+      </c>
+      <c r="C155">
+        <v>99</v>
+      </c>
+      <c r="D155">
+        <v>37</v>
+      </c>
+      <c r="E155">
+        <v>6426.86</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156">
+        <v>154</v>
+      </c>
+      <c r="B156">
+        <v>17</v>
+      </c>
+      <c r="C156">
+        <v>100</v>
+      </c>
+      <c r="D156">
+        <v>37</v>
+      </c>
+      <c r="E156">
+        <v>6448.17</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157">
+        <v>155</v>
+      </c>
+      <c r="B157">
+        <v>17</v>
+      </c>
+      <c r="C157">
+        <v>101</v>
+      </c>
+      <c r="D157">
+        <v>37</v>
+      </c>
+      <c r="E157">
+        <v>6469.46</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158">
+        <v>156</v>
+      </c>
+      <c r="B158">
+        <v>17</v>
+      </c>
+      <c r="C158">
+        <v>102</v>
+      </c>
+      <c r="D158">
+        <v>37</v>
+      </c>
+      <c r="E158">
+        <v>6490.71</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159">
+        <v>157</v>
+      </c>
+      <c r="B159">
+        <v>18</v>
+      </c>
+      <c r="C159">
+        <v>102</v>
+      </c>
+      <c r="D159">
+        <v>37</v>
+      </c>
+      <c r="E159">
+        <v>6511.95</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160">
+        <v>158</v>
+      </c>
+      <c r="B160">
+        <v>18</v>
+      </c>
+      <c r="C160">
+        <v>102</v>
+      </c>
+      <c r="D160">
+        <v>38</v>
+      </c>
+      <c r="E160">
+        <v>6533.19</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161">
+        <v>159</v>
+      </c>
+      <c r="B161">
+        <v>18</v>
+      </c>
+      <c r="C161">
+        <v>103</v>
+      </c>
+      <c r="D161">
+        <v>38</v>
+      </c>
+      <c r="E161">
+        <v>6554.41</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162">
+        <v>160</v>
+      </c>
+      <c r="B162">
+        <v>18</v>
+      </c>
+      <c r="C162">
+        <v>104</v>
+      </c>
+      <c r="D162">
+        <v>38</v>
+      </c>
+      <c r="E162">
+        <v>6575.6</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163">
+        <v>161</v>
+      </c>
+      <c r="B163">
+        <v>18</v>
+      </c>
+      <c r="C163">
+        <v>105</v>
+      </c>
+      <c r="D163">
+        <v>38</v>
+      </c>
+      <c r="E163">
+        <v>6596.76</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164">
+        <v>162</v>
+      </c>
+      <c r="B164">
+        <v>18</v>
+      </c>
+      <c r="C164">
+        <v>106</v>
+      </c>
+      <c r="D164">
+        <v>38</v>
+      </c>
+      <c r="E164">
+        <v>6617.89</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165">
+        <v>163</v>
+      </c>
+      <c r="B165">
+        <v>18</v>
+      </c>
+      <c r="C165">
+        <v>107</v>
+      </c>
+      <c r="D165">
+        <v>38</v>
+      </c>
+      <c r="E165">
+        <v>6638.99</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166">
+        <v>164</v>
+      </c>
+      <c r="B166">
+        <v>18</v>
+      </c>
+      <c r="C166">
+        <v>107</v>
+      </c>
+      <c r="D166">
+        <v>39</v>
+      </c>
+      <c r="E166">
+        <v>6660.07</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167">
+        <v>165</v>
+      </c>
+      <c r="B167">
+        <v>18</v>
+      </c>
+      <c r="C167">
+        <v>108</v>
+      </c>
+      <c r="D167">
+        <v>39</v>
+      </c>
+      <c r="E167">
+        <v>6681.14</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168">
+        <v>166</v>
+      </c>
+      <c r="B168">
+        <v>18</v>
+      </c>
+      <c r="C168">
+        <v>109</v>
+      </c>
+      <c r="D168">
+        <v>39</v>
+      </c>
+      <c r="E168">
+        <v>6702.18</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169">
+        <v>167</v>
+      </c>
+      <c r="B169">
+        <v>18</v>
+      </c>
+      <c r="C169">
+        <v>110</v>
+      </c>
+      <c r="D169">
+        <v>39</v>
+      </c>
+      <c r="E169">
+        <v>6723.19</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170">
+        <v>168</v>
+      </c>
+      <c r="B170">
+        <v>18</v>
+      </c>
+      <c r="C170">
+        <v>111</v>
+      </c>
+      <c r="D170">
+        <v>39</v>
+      </c>
+      <c r="E170">
+        <v>6744.17</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171">
+        <v>169</v>
+      </c>
+      <c r="B171">
+        <v>18</v>
+      </c>
+      <c r="C171">
+        <v>112</v>
+      </c>
+      <c r="D171">
+        <v>39</v>
+      </c>
+      <c r="E171">
+        <v>6765.13</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172">
+        <v>170</v>
+      </c>
+      <c r="B172">
+        <v>18</v>
+      </c>
+      <c r="C172">
+        <v>113</v>
+      </c>
+      <c r="D172">
+        <v>39</v>
+      </c>
+      <c r="E172">
+        <v>6786.06</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173">
+        <v>171</v>
+      </c>
+      <c r="B173">
+        <v>18</v>
+      </c>
+      <c r="C173">
+        <v>113</v>
+      </c>
+      <c r="D173">
+        <v>40</v>
+      </c>
+      <c r="E173">
+        <v>6806.97</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174">
+        <v>172</v>
+      </c>
+      <c r="B174">
+        <v>18</v>
+      </c>
+      <c r="C174">
+        <v>114</v>
+      </c>
+      <c r="D174">
+        <v>40</v>
+      </c>
+      <c r="E174">
+        <v>6827.87</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175">
+        <v>173</v>
+      </c>
+      <c r="B175">
+        <v>18</v>
+      </c>
+      <c r="C175">
+        <v>115</v>
+      </c>
+      <c r="D175">
+        <v>40</v>
+      </c>
+      <c r="E175">
+        <v>6848.74</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176">
+        <v>174</v>
+      </c>
+      <c r="B176">
+        <v>18</v>
+      </c>
+      <c r="C176">
+        <v>116</v>
+      </c>
+      <c r="D176">
+        <v>40</v>
+      </c>
+      <c r="E176">
+        <v>6869.58</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177">
+        <v>175</v>
+      </c>
+      <c r="B177">
+        <v>18</v>
+      </c>
+      <c r="C177">
+        <v>117</v>
+      </c>
+      <c r="D177">
+        <v>40</v>
+      </c>
+      <c r="E177">
+        <v>6890.4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178">
+        <v>176</v>
+      </c>
+      <c r="B178">
+        <v>18</v>
+      </c>
+      <c r="C178">
+        <v>118</v>
+      </c>
+      <c r="D178">
+        <v>40</v>
+      </c>
+      <c r="E178">
+        <v>6911.19</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179">
+        <v>177</v>
+      </c>
+      <c r="B179">
+        <v>18</v>
+      </c>
+      <c r="C179">
+        <v>119</v>
+      </c>
+      <c r="D179">
+        <v>40</v>
+      </c>
+      <c r="E179">
+        <v>6931.96</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180">
+        <v>178</v>
+      </c>
+      <c r="B180">
+        <v>18</v>
+      </c>
+      <c r="C180">
+        <v>119</v>
+      </c>
+      <c r="D180">
+        <v>41</v>
+      </c>
+      <c r="E180">
+        <v>6952.71</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181">
+        <v>179</v>
+      </c>
+      <c r="B181">
+        <v>18</v>
+      </c>
+      <c r="C181">
+        <v>120</v>
+      </c>
+      <c r="D181">
+        <v>41</v>
+      </c>
+      <c r="E181">
+        <v>6973.45</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182">
+        <v>180</v>
+      </c>
+      <c r="B182">
+        <v>19</v>
+      </c>
+      <c r="C182">
+        <v>120</v>
+      </c>
+      <c r="D182">
+        <v>41</v>
+      </c>
+      <c r="E182">
+        <v>6994.17</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183">
+        <v>181</v>
+      </c>
+      <c r="B183">
+        <v>19</v>
+      </c>
+      <c r="C183">
+        <v>121</v>
+      </c>
+      <c r="D183">
+        <v>41</v>
+      </c>
+      <c r="E183">
+        <v>7014.88</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184">
+        <v>182</v>
+      </c>
+      <c r="B184">
+        <v>19</v>
+      </c>
+      <c r="C184">
+        <v>122</v>
+      </c>
+      <c r="D184">
+        <v>41</v>
+      </c>
+      <c r="E184">
+        <v>7035.57</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185">
+        <v>183</v>
+      </c>
+      <c r="B185">
+        <v>19</v>
+      </c>
+      <c r="C185">
+        <v>123</v>
+      </c>
+      <c r="D185">
+        <v>41</v>
+      </c>
+      <c r="E185">
+        <v>7056.23</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186">
+        <v>184</v>
+      </c>
+      <c r="B186">
+        <v>19</v>
+      </c>
+      <c r="C186">
+        <v>124</v>
+      </c>
+      <c r="D186">
+        <v>41</v>
+      </c>
+      <c r="E186">
+        <v>7076.87</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187">
+        <v>185</v>
+      </c>
+      <c r="B187">
+        <v>19</v>
+      </c>
+      <c r="C187">
+        <v>125</v>
+      </c>
+      <c r="D187">
+        <v>41</v>
+      </c>
+      <c r="E187">
+        <v>7097.48</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188">
+        <v>186</v>
+      </c>
+      <c r="B188">
+        <v>19</v>
+      </c>
+      <c r="C188">
+        <v>125</v>
+      </c>
+      <c r="D188">
+        <v>42</v>
+      </c>
+      <c r="E188">
+        <v>7118.08</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189">
+        <v>187</v>
+      </c>
+      <c r="B189">
+        <v>19</v>
+      </c>
+      <c r="C189">
+        <v>126</v>
+      </c>
+      <c r="D189">
+        <v>42</v>
+      </c>
+      <c r="E189">
+        <v>7138.67</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190">
+        <v>188</v>
+      </c>
+      <c r="B190">
+        <v>19</v>
+      </c>
+      <c r="C190">
+        <v>127</v>
+      </c>
+      <c r="D190">
+        <v>42</v>
+      </c>
+      <c r="E190">
+        <v>7159.23</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191">
+        <v>189</v>
+      </c>
+      <c r="B191">
+        <v>19</v>
+      </c>
+      <c r="C191">
+        <v>128</v>
+      </c>
+      <c r="D191">
+        <v>42</v>
+      </c>
+      <c r="E191">
+        <v>7179.77</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192">
+        <v>190</v>
+      </c>
+      <c r="B192">
+        <v>19</v>
+      </c>
+      <c r="C192">
+        <v>129</v>
+      </c>
+      <c r="D192">
+        <v>42</v>
+      </c>
+      <c r="E192">
+        <v>7200.28</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193">
+        <v>191</v>
+      </c>
+      <c r="B193">
+        <v>19</v>
+      </c>
+      <c r="C193">
+        <v>130</v>
+      </c>
+      <c r="D193">
+        <v>42</v>
+      </c>
+      <c r="E193">
+        <v>7220.77</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194">
+        <v>192</v>
+      </c>
+      <c r="B194">
+        <v>19</v>
+      </c>
+      <c r="C194">
+        <v>131</v>
+      </c>
+      <c r="D194">
+        <v>42</v>
+      </c>
+      <c r="E194">
+        <v>7241.24</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195">
+        <v>193</v>
+      </c>
+      <c r="B195">
+        <v>19</v>
+      </c>
+      <c r="C195">
+        <v>131</v>
+      </c>
+      <c r="D195">
+        <v>43</v>
+      </c>
+      <c r="E195">
+        <v>7261.7</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196">
+        <v>194</v>
+      </c>
+      <c r="B196">
+        <v>19</v>
+      </c>
+      <c r="C196">
+        <v>132</v>
+      </c>
+      <c r="D196">
+        <v>43</v>
+      </c>
+      <c r="E196">
+        <v>7282.14</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197">
+        <v>195</v>
+      </c>
+      <c r="B197">
+        <v>19</v>
+      </c>
+      <c r="C197">
+        <v>133</v>
+      </c>
+      <c r="D197">
+        <v>43</v>
+      </c>
+      <c r="E197">
+        <v>7302.56</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198">
+        <v>196</v>
+      </c>
+      <c r="B198">
+        <v>19</v>
+      </c>
+      <c r="C198">
+        <v>134</v>
+      </c>
+      <c r="D198">
+        <v>43</v>
+      </c>
+      <c r="E198">
+        <v>7322.96</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199">
+        <v>197</v>
+      </c>
+      <c r="B199">
+        <v>19</v>
+      </c>
+      <c r="C199">
+        <v>135</v>
+      </c>
+      <c r="D199">
+        <v>43</v>
+      </c>
+      <c r="E199">
+        <v>7343.33</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200">
+        <v>198</v>
+      </c>
+      <c r="B200">
+        <v>19</v>
+      </c>
+      <c r="C200">
+        <v>136</v>
+      </c>
+      <c r="D200">
+        <v>43</v>
+      </c>
+      <c r="E200">
+        <v>7363.68</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201">
+        <v>199</v>
+      </c>
+      <c r="B201">
+        <v>19</v>
+      </c>
+      <c r="C201">
+        <v>137</v>
+      </c>
+      <c r="D201">
+        <v>43</v>
+      </c>
+      <c r="E201">
+        <v>7384.01</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202">
+        <v>200</v>
+      </c>
+      <c r="B202">
+        <v>19</v>
+      </c>
+      <c r="C202">
+        <v>137</v>
+      </c>
+      <c r="D202">
+        <v>44</v>
+      </c>
+      <c r="E202">
+        <v>7404.32</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203">
+        <v>201</v>
+      </c>
+      <c r="B203">
+        <v>19</v>
+      </c>
+      <c r="C203">
+        <v>138</v>
+      </c>
+      <c r="D203">
+        <v>44</v>
+      </c>
+      <c r="E203">
+        <v>7424.63</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204">
+        <v>202</v>
+      </c>
+      <c r="B204">
+        <v>19</v>
+      </c>
+      <c r="C204">
+        <v>139</v>
+      </c>
+      <c r="D204">
+        <v>44</v>
+      </c>
+      <c r="E204">
+        <v>7444.92</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205">
+        <v>203</v>
+      </c>
+      <c r="B205">
+        <v>19</v>
+      </c>
+      <c r="C205">
+        <v>140</v>
+      </c>
+      <c r="D205">
+        <v>44</v>
+      </c>
+      <c r="E205">
+        <v>7465.18</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206">
+        <v>204</v>
+      </c>
+      <c r="B206">
+        <v>19</v>
+      </c>
+      <c r="C206">
+        <v>141</v>
+      </c>
+      <c r="D206">
+        <v>44</v>
+      </c>
+      <c r="E206">
+        <v>7485.42</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207">
+        <v>205</v>
+      </c>
+      <c r="B207">
+        <v>20</v>
+      </c>
+      <c r="C207">
+        <v>141</v>
+      </c>
+      <c r="D207">
+        <v>44</v>
+      </c>
+      <c r="E207">
+        <v>7505.65</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208">
+        <v>206</v>
+      </c>
+      <c r="B208">
+        <v>20</v>
+      </c>
+      <c r="C208">
+        <v>142</v>
+      </c>
+      <c r="D208">
+        <v>44</v>
+      </c>
+      <c r="E208">
+        <v>7525.87</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209">
+        <v>207</v>
+      </c>
+      <c r="B209">
+        <v>20</v>
+      </c>
+      <c r="C209">
+        <v>143</v>
+      </c>
+      <c r="D209">
+        <v>44</v>
+      </c>
+      <c r="E209">
+        <v>7546.07</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210">
+        <v>208</v>
+      </c>
+      <c r="B210">
+        <v>20</v>
+      </c>
+      <c r="C210">
+        <v>144</v>
+      </c>
+      <c r="D210">
+        <v>44</v>
+      </c>
+      <c r="E210">
+        <v>7566.25</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211">
+        <v>209</v>
+      </c>
+      <c r="B211">
+        <v>20</v>
+      </c>
+      <c r="C211">
+        <v>144</v>
+      </c>
+      <c r="D211">
+        <v>45</v>
+      </c>
+      <c r="E211">
+        <v>7586.42</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212">
+        <v>210</v>
+      </c>
+      <c r="B212">
+        <v>20</v>
+      </c>
+      <c r="C212">
+        <v>145</v>
+      </c>
+      <c r="D212">
+        <v>45</v>
+      </c>
+      <c r="E212">
+        <v>7606.58</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213">
+        <v>211</v>
+      </c>
+      <c r="B213">
+        <v>20</v>
+      </c>
+      <c r="C213">
+        <v>146</v>
+      </c>
+      <c r="D213">
+        <v>45</v>
+      </c>
+      <c r="E213">
+        <v>7626.71</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214">
+        <v>212</v>
+      </c>
+      <c r="B214">
+        <v>20</v>
+      </c>
+      <c r="C214">
+        <v>147</v>
+      </c>
+      <c r="D214">
+        <v>45</v>
+      </c>
+      <c r="E214">
+        <v>7646.83</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215">
+        <v>213</v>
+      </c>
+      <c r="B215">
+        <v>20</v>
+      </c>
+      <c r="C215">
+        <v>148</v>
+      </c>
+      <c r="D215">
+        <v>45</v>
+      </c>
+      <c r="E215">
+        <v>7666.92</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216">
+        <v>214</v>
+      </c>
+      <c r="B216">
+        <v>20</v>
+      </c>
+      <c r="C216">
+        <v>149</v>
+      </c>
+      <c r="D216">
+        <v>45</v>
+      </c>
+      <c r="E216">
+        <v>7687</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217">
+        <v>215</v>
+      </c>
+      <c r="B217">
+        <v>20</v>
+      </c>
+      <c r="C217">
+        <v>150</v>
+      </c>
+      <c r="D217">
+        <v>45</v>
+      </c>
+      <c r="E217">
+        <v>7707.05</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="A218">
+        <v>216</v>
+      </c>
+      <c r="B218">
+        <v>20</v>
+      </c>
+      <c r="C218">
+        <v>150</v>
+      </c>
+      <c r="D218">
+        <v>46</v>
+      </c>
+      <c r="E218">
+        <v>7727.09</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219">
+        <v>217</v>
+      </c>
+      <c r="B219">
+        <v>20</v>
+      </c>
+      <c r="C219">
+        <v>151</v>
+      </c>
+      <c r="D219">
+        <v>46</v>
+      </c>
+      <c r="E219">
+        <v>7747.13</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220">
+        <v>218</v>
+      </c>
+      <c r="B220">
+        <v>20</v>
+      </c>
+      <c r="C220">
+        <v>152</v>
+      </c>
+      <c r="D220">
+        <v>46</v>
+      </c>
+      <c r="E220">
+        <v>7767.14</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221">
+        <v>219</v>
+      </c>
+      <c r="B221">
+        <v>20</v>
+      </c>
+      <c r="C221">
+        <v>153</v>
+      </c>
+      <c r="D221">
+        <v>46</v>
+      </c>
+      <c r="E221">
+        <v>7787.13</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
+      <c r="A222">
+        <v>220</v>
+      </c>
+      <c r="B222">
+        <v>20</v>
+      </c>
+      <c r="C222">
+        <v>154</v>
+      </c>
+      <c r="D222">
+        <v>46</v>
+      </c>
+      <c r="E222">
+        <v>7807.11</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
+      <c r="A223">
+        <v>221</v>
+      </c>
+      <c r="B223">
+        <v>20</v>
+      </c>
+      <c r="C223">
+        <v>155</v>
+      </c>
+      <c r="D223">
+        <v>46</v>
+      </c>
+      <c r="E223">
+        <v>7827.06</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="A224">
+        <v>222</v>
+      </c>
+      <c r="B224">
+        <v>20</v>
+      </c>
+      <c r="C224">
+        <v>156</v>
+      </c>
+      <c r="D224">
+        <v>46</v>
+      </c>
+      <c r="E224">
+        <v>7847</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
+      <c r="A225">
+        <v>223</v>
+      </c>
+      <c r="B225">
+        <v>20</v>
+      </c>
+      <c r="C225">
+        <v>157</v>
+      </c>
+      <c r="D225">
+        <v>46</v>
+      </c>
+      <c r="E225">
+        <v>7866.92</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5">
+      <c r="A226">
+        <v>224</v>
+      </c>
+      <c r="B226">
+        <v>20</v>
+      </c>
+      <c r="C226">
+        <v>157</v>
+      </c>
+      <c r="D226">
+        <v>47</v>
+      </c>
+      <c r="E226">
+        <v>7886.83</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
+      <c r="A227">
+        <v>225</v>
+      </c>
+      <c r="B227">
+        <v>20</v>
+      </c>
+      <c r="C227">
+        <v>158</v>
+      </c>
+      <c r="D227">
+        <v>47</v>
+      </c>
+      <c r="E227">
+        <v>7906.72</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
+      <c r="A228">
+        <v>226</v>
+      </c>
+      <c r="B228">
+        <v>20</v>
+      </c>
+      <c r="C228">
+        <v>159</v>
+      </c>
+      <c r="D228">
+        <v>47</v>
+      </c>
+      <c r="E228">
+        <v>7926.6</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
+      <c r="A229">
+        <v>227</v>
+      </c>
+      <c r="B229">
+        <v>20</v>
+      </c>
+      <c r="C229">
+        <v>160</v>
+      </c>
+      <c r="D229">
+        <v>47</v>
+      </c>
+      <c r="E229">
+        <v>7946.46</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
+      <c r="A230">
+        <v>228</v>
+      </c>
+      <c r="B230">
+        <v>20</v>
+      </c>
+      <c r="C230">
+        <v>161</v>
+      </c>
+      <c r="D230">
+        <v>47</v>
+      </c>
+      <c r="E230">
+        <v>7966.3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5">
+      <c r="A231">
+        <v>229</v>
+      </c>
+      <c r="B231">
+        <v>20</v>
+      </c>
+      <c r="C231">
+        <v>162</v>
+      </c>
+      <c r="D231">
+        <v>47</v>
+      </c>
+      <c r="E231">
+        <v>7986.13</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="A232">
+        <v>230</v>
+      </c>
+      <c r="B232">
+        <v>20</v>
+      </c>
+      <c r="C232">
+        <v>163</v>
+      </c>
+      <c r="D232">
+        <v>47</v>
+      </c>
+      <c r="E232">
+        <v>8005.93</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
+      <c r="A233">
+        <v>231</v>
+      </c>
+      <c r="B233">
+        <v>20</v>
+      </c>
+      <c r="C233">
+        <v>164</v>
+      </c>
+      <c r="D233">
+        <v>47</v>
+      </c>
+      <c r="E233">
+        <v>8025.72</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5">
+      <c r="A234">
+        <v>232</v>
+      </c>
+      <c r="B234">
+        <v>20</v>
+      </c>
+      <c r="C234">
+        <v>164</v>
+      </c>
+      <c r="D234">
+        <v>48</v>
+      </c>
+      <c r="E234">
+        <v>8045.5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5">
+      <c r="A235">
+        <v>233</v>
+      </c>
+      <c r="B235">
+        <v>21</v>
+      </c>
+      <c r="C235">
+        <v>164</v>
+      </c>
+      <c r="D235">
+        <v>48</v>
+      </c>
+      <c r="E235">
+        <v>8065.28</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5">
+      <c r="A236">
+        <v>234</v>
+      </c>
+      <c r="B236">
+        <v>21</v>
+      </c>
+      <c r="C236">
+        <v>165</v>
+      </c>
+      <c r="D236">
+        <v>48</v>
+      </c>
+      <c r="E236">
+        <v>8085.05</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
+      <c r="A237">
+        <v>235</v>
+      </c>
+      <c r="B237">
+        <v>21</v>
+      </c>
+      <c r="C237">
+        <v>166</v>
+      </c>
+      <c r="D237">
+        <v>48</v>
+      </c>
+      <c r="E237">
+        <v>8104.8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5">
+      <c r="A238">
+        <v>236</v>
+      </c>
+      <c r="B238">
+        <v>21</v>
+      </c>
+      <c r="C238">
+        <v>167</v>
+      </c>
+      <c r="D238">
+        <v>48</v>
+      </c>
+      <c r="E238">
+        <v>8124.53</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5">
+      <c r="A239">
+        <v>237</v>
+      </c>
+      <c r="B239">
+        <v>21</v>
+      </c>
+      <c r="C239">
+        <v>168</v>
+      </c>
+      <c r="D239">
+        <v>48</v>
+      </c>
+      <c r="E239">
+        <v>8144.25</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="A240">
+        <v>238</v>
+      </c>
+      <c r="B240">
+        <v>21</v>
+      </c>
+      <c r="C240">
+        <v>169</v>
+      </c>
+      <c r="D240">
+        <v>48</v>
+      </c>
+      <c r="E240">
+        <v>8163.94</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
+      <c r="A241">
+        <v>239</v>
+      </c>
+      <c r="B241">
+        <v>21</v>
+      </c>
+      <c r="C241">
+        <v>170</v>
+      </c>
+      <c r="D241">
+        <v>48</v>
+      </c>
+      <c r="E241">
+        <v>8183.62</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5">
+      <c r="A242">
+        <v>240</v>
+      </c>
+      <c r="B242">
+        <v>21</v>
+      </c>
+      <c r="C242">
+        <v>171</v>
+      </c>
+      <c r="D242">
+        <v>48</v>
+      </c>
+      <c r="E242">
+        <v>8203.290000000001</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
+      <c r="A243">
+        <v>241</v>
+      </c>
+      <c r="B243">
+        <v>21</v>
+      </c>
+      <c r="C243">
+        <v>171</v>
+      </c>
+      <c r="D243">
+        <v>49</v>
+      </c>
+      <c r="E243">
+        <v>8222.950000000001</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
+      <c r="A244">
+        <v>242</v>
+      </c>
+      <c r="B244">
+        <v>21</v>
+      </c>
+      <c r="C244">
+        <v>172</v>
+      </c>
+      <c r="D244">
+        <v>49</v>
+      </c>
+      <c r="E244">
+        <v>8242.59</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5">
+      <c r="A245">
+        <v>243</v>
+      </c>
+      <c r="B245">
+        <v>21</v>
+      </c>
+      <c r="C245">
+        <v>173</v>
+      </c>
+      <c r="D245">
+        <v>49</v>
+      </c>
+      <c r="E245">
+        <v>8262.219999999999</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5">
+      <c r="A246">
+        <v>244</v>
+      </c>
+      <c r="B246">
+        <v>21</v>
+      </c>
+      <c r="C246">
+        <v>174</v>
+      </c>
+      <c r="D246">
+        <v>49</v>
+      </c>
+      <c r="E246">
+        <v>8281.83</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
+      <c r="A247">
+        <v>245</v>
+      </c>
+      <c r="B247">
+        <v>21</v>
+      </c>
+      <c r="C247">
+        <v>175</v>
+      </c>
+      <c r="D247">
+        <v>49</v>
+      </c>
+      <c r="E247">
+        <v>8301.42</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5">
+      <c r="A248">
+        <v>246</v>
+      </c>
+      <c r="B248">
+        <v>21</v>
+      </c>
+      <c r="C248">
+        <v>176</v>
+      </c>
+      <c r="D248">
+        <v>49</v>
+      </c>
+      <c r="E248">
+        <v>8321</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
+      <c r="A249">
+        <v>247</v>
+      </c>
+      <c r="B249">
+        <v>21</v>
+      </c>
+      <c r="C249">
+        <v>177</v>
+      </c>
+      <c r="D249">
+        <v>49</v>
+      </c>
+      <c r="E249">
+        <v>8340.559999999999</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5">
+      <c r="A250">
+        <v>248</v>
+      </c>
+      <c r="B250">
+        <v>21</v>
+      </c>
+      <c r="C250">
+        <v>178</v>
+      </c>
+      <c r="D250">
+        <v>49</v>
+      </c>
+      <c r="E250">
+        <v>8360.110000000001</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5">
+      <c r="A251">
+        <v>249</v>
+      </c>
+      <c r="B251">
+        <v>21</v>
+      </c>
+      <c r="C251">
+        <v>178</v>
+      </c>
+      <c r="D251">
+        <v>50</v>
+      </c>
+      <c r="E251">
+        <v>8379.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>